<commit_message>
added cache time & auto refresh
</commit_message>
<xml_diff>
--- a/dashboard/Book1.xlsx
+++ b/dashboard/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tajdi\Documents\tauri-app\dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4060C312-35C4-4E80-8236-44B6F2A87BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095B24DC-1E3F-41E2-82BA-619E4C12A659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{068C44D0-5624-4079-B1C8-28F77F23031C}"/>
   </bookViews>
@@ -410,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C6A88F-53E4-49F8-BDA0-729F89C77E58}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,6 +438,36 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>